<commit_message>
Trabajando en manejo de errores y realizando pruebas reales de uso
</commit_message>
<xml_diff>
--- a/excel/32158(top).xlsx
+++ b/excel/32158(top).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_1F0F507C57CC8D1C9424A318C64930BBDF704713" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48A39D6A-80A4-4336-B208-9DF7490CC063}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_1F0F507C57CC8D1C9424A318C64930BBDF704713" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD56356E-3093-47A7-AB4F-C2548BDF23EB}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="360" windowWidth="14400" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$547</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E513" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +898,7 @@
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -939,7 +939,7 @@
         <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3" t="s">
         <v>20</v>
@@ -974,7 +974,7 @@
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O4" t="s">
         <v>20</v>
@@ -1009,7 +1009,7 @@
         <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -1050,7 +1050,7 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
         <v>21</v>
@@ -1091,7 +1091,7 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O7" t="s">
         <v>20</v>
@@ -1126,7 +1126,7 @@
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
         <v>21</v>
@@ -1167,7 +1167,7 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
         <v>21</v>
@@ -1208,7 +1208,7 @@
         <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
@@ -1249,7 +1249,7 @@
         <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
         <v>21</v>
@@ -20005,7 +20005,7 @@
         <v>19</v>
       </c>
       <c r="I503" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O503" t="s">
         <v>20</v>
@@ -20573,7 +20573,7 @@
         <v>19</v>
       </c>
       <c r="I517" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O517" t="s">
         <v>20</v>
@@ -20608,7 +20608,7 @@
         <v>19</v>
       </c>
       <c r="I518" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O518" t="s">
         <v>20</v>
@@ -20684,7 +20684,7 @@
         <v>19</v>
       </c>
       <c r="I520" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O520" t="s">
         <v>20</v>
@@ -21088,7 +21088,7 @@
         <v>19</v>
       </c>
       <c r="I530" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O530" t="s">
         <v>20</v>
@@ -21123,7 +21123,7 @@
         <v>19</v>
       </c>
       <c r="I531" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O531" t="s">
         <v>20</v>
@@ -21158,7 +21158,7 @@
         <v>19</v>
       </c>
       <c r="I532" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O532" t="s">
         <v>20</v>
@@ -21193,7 +21193,7 @@
         <v>19</v>
       </c>
       <c r="I533" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O533" t="s">
         <v>20</v>
@@ -21392,7 +21392,7 @@
         <v>19</v>
       </c>
       <c r="I538" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O538" t="s">
         <v>20</v>
@@ -21427,7 +21427,7 @@
         <v>19</v>
       </c>
       <c r="I539" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O539" t="s">
         <v>20</v>
@@ -21503,7 +21503,7 @@
         <v>19</v>
       </c>
       <c r="I541" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O541" t="s">
         <v>20</v>
@@ -21538,7 +21538,7 @@
         <v>19</v>
       </c>
       <c r="I542" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O542" t="s">
         <v>20</v>
@@ -21614,7 +21614,7 @@
         <v>19</v>
       </c>
       <c r="I544" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O544" t="s">
         <v>20</v>
@@ -21750,6 +21750,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:Q1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Despliegue de app a produccion para testeos,una vez validad se aplicaran cambios pertinentes y se dara por finaliazdo el proyecto
</commit_message>
<xml_diff>
--- a/excel/32158(top).xlsx
+++ b/excel/32158(top).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_1F0F507C57CC8D1C9424A318C64930BBDF704713" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD56356E-3093-47A7-AB4F-C2548BDF23EB}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_1F0F507C57CC8D1C9424A318C64930BBDF704713" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F1C56DF-0C89-4C45-BBAE-D91AE4B68E7D}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="360" windowWidth="14400" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14415" yWindow="1200" windowWidth="14385" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -814,7 +814,7 @@
   <dimension ref="A1:Q547"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +898,7 @@
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -939,7 +939,7 @@
         <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O3" t="s">
         <v>20</v>
@@ -974,7 +974,7 @@
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O4" t="s">
         <v>20</v>
@@ -1009,7 +1009,7 @@
         <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -1050,7 +1050,7 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
         <v>21</v>
@@ -1091,7 +1091,7 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O7" t="s">
         <v>20</v>
@@ -1126,7 +1126,7 @@
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
         <v>21</v>
@@ -1167,7 +1167,7 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" t="s">
         <v>21</v>
@@ -1208,7 +1208,7 @@
         <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
@@ -1249,7 +1249,7 @@
         <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" t="s">
         <v>21</v>

</xml_diff>